<commit_message>
Working Model including ITS
</commit_message>
<xml_diff>
--- a/Outputs/WY/CausalImpact/Results.xlsx
+++ b/Outputs/WY/CausalImpact/Results.xlsx
@@ -437,16 +437,16 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>4.49434704126458</v>
+        <v>4.4620803418763</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.0200647407029696</v>
+        <v>0.0487316900224034</v>
       </c>
       <c r="F2" t="n">
-        <v>9.38944431520974</v>
+        <v>9.17324141384519</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
         <v>1572.84210526316</v>
@@ -466,13 +466,13 @@
         <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.95048540473244</v>
+        <v>-1.94436936968067</v>
       </c>
       <c r="E3" t="n">
-        <v>-13.1664060622003</v>
+        <v>-13.528432402614</v>
       </c>
       <c r="F3" t="n">
-        <v>11.6063619007748</v>
+        <v>12.3223813947637</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -495,13 +495,13 @@
         <v>13</v>
       </c>
       <c r="D4" t="n">
-        <v>-7.09122497395407</v>
+        <v>-6.86483921876909</v>
       </c>
       <c r="E4" t="n">
-        <v>-15.8122405849142</v>
+        <v>-15.8793496859715</v>
       </c>
       <c r="F4" t="n">
-        <v>3.48785810902259</v>
+        <v>4.49968362782727</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -524,13 +524,13 @@
         <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.26620263224843</v>
+        <v>-1.0734231285165</v>
       </c>
       <c r="E5" t="n">
-        <v>-18.221918326023</v>
+        <v>-18.292886636882</v>
       </c>
       <c r="F5" t="n">
-        <v>20.6780261026954</v>
+        <v>18.9355016824991</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -553,13 +553,13 @@
         <v>15</v>
       </c>
       <c r="D6" t="n">
-        <v>-46.021338074079</v>
+        <v>-45.8161278523735</v>
       </c>
       <c r="E6" t="n">
-        <v>-52.4543529578244</v>
+        <v>-52.4625948548407</v>
       </c>
       <c r="F6" t="n">
-        <v>-38.1587394898575</v>
+        <v>-38.0371930503741</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -582,13 +582,13 @@
         <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>20.4110468700689</v>
+        <v>20.310687173548</v>
       </c>
       <c r="E7" t="n">
-        <v>13.1031899553703</v>
+        <v>12.7696283939118</v>
       </c>
       <c r="F7" t="n">
-        <v>28.6185945240833</v>
+        <v>28.2935380333947</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -611,13 +611,13 @@
         <v>12</v>
       </c>
       <c r="D8" t="n">
-        <v>21.1132101320975</v>
+        <v>20.9120697187212</v>
       </c>
       <c r="E8" t="n">
-        <v>12.031340198246</v>
+        <v>11.3063218609538</v>
       </c>
       <c r="F8" t="n">
-        <v>31.4158442583437</v>
+        <v>31.7074286495627</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
@@ -640,13 +640,13 @@
         <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>58.1573589263004</v>
+        <v>57.7048358712487</v>
       </c>
       <c r="E9" t="n">
-        <v>32.2420163991034</v>
+        <v>30.1121102994413</v>
       </c>
       <c r="F9" t="n">
-        <v>93.2084262339504</v>
+        <v>92.6300489366462</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -669,13 +669,13 @@
         <v>14</v>
       </c>
       <c r="D10" t="n">
-        <v>56.2617951937859</v>
+        <v>56.2263396253209</v>
       </c>
       <c r="E10" t="n">
-        <v>30.4453155572539</v>
+        <v>28.9858016511982</v>
       </c>
       <c r="F10" t="n">
-        <v>91.8638718981945</v>
+        <v>95.0920997190956</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
@@ -698,13 +698,13 @@
         <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>-16.7226258689706</v>
+        <v>-16.7221882581324</v>
       </c>
       <c r="E11" t="n">
-        <v>-24.8436211934526</v>
+        <v>-25.4740557857607</v>
       </c>
       <c r="F11" t="n">
-        <v>-6.32981996256163</v>
+        <v>-6.87793350549224</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
@@ -727,13 +727,13 @@
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>3.41743793543934</v>
+        <v>3.42926773014022</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.733696936857492</v>
+        <v>-0.649730002167931</v>
       </c>
       <c r="F12" t="n">
-        <v>8.16179723002123</v>
+        <v>7.9168602605143</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -756,13 +756,13 @@
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>19.4908017364961</v>
+        <v>19.717269776304</v>
       </c>
       <c r="E13" t="n">
-        <v>7.39102360485247</v>
+        <v>7.64556013582691</v>
       </c>
       <c r="F13" t="n">
-        <v>32.8229791746086</v>
+        <v>34.1580900871777</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -785,13 +785,13 @@
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>122.185541063488</v>
+        <v>119.941233146547</v>
       </c>
       <c r="E14" t="n">
-        <v>62.9908810278721</v>
+        <v>64.0966515107077</v>
       </c>
       <c r="F14" t="n">
-        <v>215.527702818509</v>
+        <v>212.337419169173</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -814,13 +814,13 @@
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>203.738978149121</v>
+        <v>205.336789972671</v>
       </c>
       <c r="E15" t="n">
-        <v>99.3877550182712</v>
+        <v>99.8184481009487</v>
       </c>
       <c r="F15" t="n">
-        <v>400.477940302165</v>
+        <v>403.467035329428</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
@@ -843,13 +843,13 @@
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>145.615709550592</v>
+        <v>146.866805185933</v>
       </c>
       <c r="E16" t="n">
-        <v>82.2634257361837</v>
+        <v>85.6710881283994</v>
       </c>
       <c r="F16" t="n">
-        <v>238.324684889548</v>
+        <v>244.687752334718</v>
       </c>
       <c r="G16" t="n">
         <v>1</v>
@@ -872,13 +872,13 @@
         <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>4.01154034205972</v>
+        <v>4.04281806643453</v>
       </c>
       <c r="E17" t="n">
-        <v>0.892250819928284</v>
+        <v>0.854746669993673</v>
       </c>
       <c r="F17" t="n">
-        <v>7.31897108918148</v>
+        <v>7.53884418729428</v>
       </c>
       <c r="G17" t="n">
         <v>1</v>
@@ -901,13 +901,13 @@
         <v>12</v>
       </c>
       <c r="D18" t="n">
-        <v>21.8731637098883</v>
+        <v>21.7792733865914</v>
       </c>
       <c r="E18" t="n">
-        <v>12.6664066799996</v>
+        <v>14.0776701889269</v>
       </c>
       <c r="F18" t="n">
-        <v>31.7019139104026</v>
+        <v>31.3177937331251</v>
       </c>
       <c r="G18" t="n">
         <v>1</v>
@@ -930,13 +930,13 @@
         <v>13</v>
       </c>
       <c r="D19" t="n">
-        <v>76.0650555841452</v>
+        <v>75.4664393431562</v>
       </c>
       <c r="E19" t="n">
-        <v>53.8052677428298</v>
+        <v>52.6867297592668</v>
       </c>
       <c r="F19" t="n">
-        <v>102.650787883898</v>
+        <v>106.762433359726</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
@@ -959,13 +959,13 @@
         <v>14</v>
       </c>
       <c r="D20" t="n">
-        <v>67.2239279584828</v>
+        <v>67.9517920871551</v>
       </c>
       <c r="E20" t="n">
-        <v>32.1406290172119</v>
+        <v>32.0786288686597</v>
       </c>
       <c r="F20" t="n">
-        <v>124.909290030572</v>
+        <v>118.261046221184</v>
       </c>
       <c r="G20" t="n">
         <v>1</v>
@@ -988,13 +988,13 @@
         <v>15</v>
       </c>
       <c r="D21" t="n">
-        <v>-43.4326458028163</v>
+        <v>-43.5048466077246</v>
       </c>
       <c r="E21" t="n">
-        <v>-48.7695166389755</v>
+        <v>-48.730212751521</v>
       </c>
       <c r="F21" t="n">
-        <v>-36.9951396011542</v>
+        <v>-36.8311276706547</v>
       </c>
       <c r="G21" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Code set up for two main models
</commit_message>
<xml_diff>
--- a/Outputs/WY/CausalImpact/Results.xlsx
+++ b/Outputs/WY/CausalImpact/Results.xlsx
@@ -437,13 +437,13 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>4.4620803418763</v>
+        <v>4.4506355143153</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0487316900224034</v>
+        <v>0.00285604647398976</v>
       </c>
       <c r="F2" t="n">
-        <v>9.17324141384519</v>
+        <v>9.02494084158365</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -466,13 +466,13 @@
         <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.94436936968067</v>
+        <v>-2.11609378373202</v>
       </c>
       <c r="E3" t="n">
-        <v>-13.528432402614</v>
+        <v>-12.8883611485623</v>
       </c>
       <c r="F3" t="n">
-        <v>12.3223813947637</v>
+        <v>11.59381101243</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -495,13 +495,13 @@
         <v>13</v>
       </c>
       <c r="D4" t="n">
-        <v>-6.86483921876909</v>
+        <v>-7.00930374180072</v>
       </c>
       <c r="E4" t="n">
-        <v>-15.8793496859715</v>
+        <v>-16.6027367891976</v>
       </c>
       <c r="F4" t="n">
-        <v>4.49968362782727</v>
+        <v>4.28883999589752</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -524,13 +524,13 @@
         <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.0734231285165</v>
+        <v>-1.74184002624819</v>
       </c>
       <c r="E5" t="n">
-        <v>-18.292886636882</v>
+        <v>-18.2670179550036</v>
       </c>
       <c r="F5" t="n">
-        <v>18.9355016824991</v>
+        <v>22.7364232948649</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -553,13 +553,13 @@
         <v>15</v>
       </c>
       <c r="D6" t="n">
-        <v>-45.8161278523735</v>
+        <v>-45.9509661291549</v>
       </c>
       <c r="E6" t="n">
-        <v>-52.4625948548407</v>
+        <v>-52.2370300644955</v>
       </c>
       <c r="F6" t="n">
-        <v>-38.0371930503741</v>
+        <v>-38.0131824436994</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -582,13 +582,13 @@
         <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>20.310687173548</v>
+        <v>20.2234112958771</v>
       </c>
       <c r="E7" t="n">
-        <v>12.7696283939118</v>
+        <v>12.7463208602078</v>
       </c>
       <c r="F7" t="n">
-        <v>28.2935380333947</v>
+        <v>28.108498415062</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -611,13 +611,13 @@
         <v>12</v>
       </c>
       <c r="D8" t="n">
-        <v>20.9120697187212</v>
+        <v>21.2087247003941</v>
       </c>
       <c r="E8" t="n">
-        <v>11.3063218609538</v>
+        <v>10.901569176131</v>
       </c>
       <c r="F8" t="n">
-        <v>31.7074286495627</v>
+        <v>31.5510611421812</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
@@ -640,13 +640,13 @@
         <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>57.7048358712487</v>
+        <v>57.9766805011587</v>
       </c>
       <c r="E9" t="n">
-        <v>30.1121102994413</v>
+        <v>31.6400838022658</v>
       </c>
       <c r="F9" t="n">
-        <v>92.6300489366462</v>
+        <v>95.9139171081479</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -669,13 +669,13 @@
         <v>14</v>
       </c>
       <c r="D10" t="n">
-        <v>56.2263396253209</v>
+        <v>56.5810737412604</v>
       </c>
       <c r="E10" t="n">
-        <v>28.9858016511982</v>
+        <v>30.3455798234838</v>
       </c>
       <c r="F10" t="n">
-        <v>95.0920997190956</v>
+        <v>98.506311160116</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
@@ -698,13 +698,13 @@
         <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>-16.7221882581324</v>
+        <v>-16.8657393725726</v>
       </c>
       <c r="E11" t="n">
-        <v>-25.4740557857607</v>
+        <v>-25.1307165779118</v>
       </c>
       <c r="F11" t="n">
-        <v>-6.87793350549224</v>
+        <v>-6.77511780061891</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
@@ -727,13 +727,13 @@
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>3.42926773014022</v>
+        <v>3.43294638693178</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.649730002167931</v>
+        <v>-0.65012984413163</v>
       </c>
       <c r="F12" t="n">
-        <v>7.9168602605143</v>
+        <v>7.76134619583574</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -756,13 +756,13 @@
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>19.717269776304</v>
+        <v>19.8472512305629</v>
       </c>
       <c r="E13" t="n">
-        <v>7.64556013582691</v>
+        <v>6.69157486838403</v>
       </c>
       <c r="F13" t="n">
-        <v>34.1580900871777</v>
+        <v>34.1299304695193</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -785,13 +785,13 @@
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>119.941233146547</v>
+        <v>120.130500317897</v>
       </c>
       <c r="E14" t="n">
-        <v>64.0966515107077</v>
+        <v>63.7314956449412</v>
       </c>
       <c r="F14" t="n">
-        <v>212.337419169173</v>
+        <v>214.822381699593</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -814,13 +814,13 @@
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>205.336789972671</v>
+        <v>210.557828156942</v>
       </c>
       <c r="E15" t="n">
-        <v>99.8184481009487</v>
+        <v>97.0460216264289</v>
       </c>
       <c r="F15" t="n">
-        <v>403.467035329428</v>
+        <v>398.826930346321</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
@@ -843,13 +843,13 @@
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>146.866805185933</v>
+        <v>145.771235644729</v>
       </c>
       <c r="E16" t="n">
-        <v>85.6710881283994</v>
+        <v>83.5447401488224</v>
       </c>
       <c r="F16" t="n">
-        <v>244.687752334718</v>
+        <v>230.641682750723</v>
       </c>
       <c r="G16" t="n">
         <v>1</v>
@@ -872,13 +872,13 @@
         <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>4.04281806643453</v>
+        <v>4.07448859494469</v>
       </c>
       <c r="E17" t="n">
-        <v>0.854746669993673</v>
+        <v>0.839500229598382</v>
       </c>
       <c r="F17" t="n">
-        <v>7.53884418729428</v>
+        <v>7.50010627375154</v>
       </c>
       <c r="G17" t="n">
         <v>1</v>
@@ -901,13 +901,13 @@
         <v>12</v>
       </c>
       <c r="D18" t="n">
-        <v>21.7792733865914</v>
+        <v>21.9194187208039</v>
       </c>
       <c r="E18" t="n">
-        <v>14.0776701889269</v>
+        <v>13.9518720111582</v>
       </c>
       <c r="F18" t="n">
-        <v>31.3177937331251</v>
+        <v>31.3962266751789</v>
       </c>
       <c r="G18" t="n">
         <v>1</v>
@@ -930,13 +930,13 @@
         <v>13</v>
       </c>
       <c r="D19" t="n">
-        <v>75.4664393431562</v>
+        <v>76.7214989760613</v>
       </c>
       <c r="E19" t="n">
-        <v>52.6867297592668</v>
+        <v>53.4462798150482</v>
       </c>
       <c r="F19" t="n">
-        <v>106.762433359726</v>
+        <v>105.219584370388</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
@@ -959,13 +959,13 @@
         <v>14</v>
       </c>
       <c r="D20" t="n">
-        <v>67.9517920871551</v>
+        <v>66.9266910978088</v>
       </c>
       <c r="E20" t="n">
-        <v>32.0786288686597</v>
+        <v>31.2964152129587</v>
       </c>
       <c r="F20" t="n">
-        <v>118.261046221184</v>
+        <v>117.638330980901</v>
       </c>
       <c r="G20" t="n">
         <v>1</v>
@@ -988,13 +988,13 @@
         <v>15</v>
       </c>
       <c r="D21" t="n">
-        <v>-43.5048466077246</v>
+        <v>-43.4121490548788</v>
       </c>
       <c r="E21" t="n">
-        <v>-48.730212751521</v>
+        <v>-48.6899213714106</v>
       </c>
       <c r="F21" t="n">
-        <v>-36.8311276706547</v>
+        <v>-36.7459298937381</v>
       </c>
       <c r="G21" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Analysis now controlling for new referals and incomplete pathways, seasonality and bed occupancy
</commit_message>
<xml_diff>
--- a/Outputs/WY/CausalImpact/Results.xlsx
+++ b/Outputs/WY/CausalImpact/Results.xlsx
@@ -437,16 +437,16 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>4.4506355143153</v>
+        <v>3.37684444861195</v>
       </c>
       <c r="E2" t="n">
-        <v>0.00285604647398976</v>
+        <v>-5.13856388713722</v>
       </c>
       <c r="F2" t="n">
-        <v>9.02494084158365</v>
+        <v>8.99158073420979</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>1572.84210526316</v>
@@ -466,16 +466,16 @@
         <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>-2.11609378373202</v>
+        <v>-22.8676613737711</v>
       </c>
       <c r="E3" t="n">
-        <v>-12.8883611485623</v>
+        <v>-32.2795665879931</v>
       </c>
       <c r="F3" t="n">
-        <v>11.59381101243</v>
+        <v>-4.42070723999729</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
         <v>271.789473684211</v>
@@ -495,16 +495,16 @@
         <v>13</v>
       </c>
       <c r="D4" t="n">
-        <v>-7.00930374180072</v>
+        <v>-27.7906514053958</v>
       </c>
       <c r="E4" t="n">
-        <v>-16.6027367891976</v>
+        <v>-38.3265017488862</v>
       </c>
       <c r="F4" t="n">
-        <v>4.28883999589752</v>
+        <v>-6.52843663571799</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>67.1052631578947</v>
@@ -524,13 +524,13 @@
         <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.74184002624819</v>
+        <v>-23.1946597042139</v>
       </c>
       <c r="E5" t="n">
-        <v>-18.2670179550036</v>
+        <v>-63.3923204252342</v>
       </c>
       <c r="F5" t="n">
-        <v>22.7364232948649</v>
+        <v>25.4145741152583</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -553,13 +553,13 @@
         <v>15</v>
       </c>
       <c r="D6" t="n">
-        <v>-45.9509661291549</v>
+        <v>-44.8432635071778</v>
       </c>
       <c r="E6" t="n">
-        <v>-52.2370300644955</v>
+        <v>-53.3608177086025</v>
       </c>
       <c r="F6" t="n">
-        <v>-38.0131824436994</v>
+        <v>-36.7757597793092</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -582,16 +582,16 @@
         <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>20.2234112958771</v>
+        <v>1.12243934249334</v>
       </c>
       <c r="E7" t="n">
-        <v>12.7463208602078</v>
+        <v>-11.2347177065196</v>
       </c>
       <c r="F7" t="n">
-        <v>28.108498415062</v>
+        <v>15.1138482931335</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>3171.42105263158</v>
@@ -611,16 +611,16 @@
         <v>12</v>
       </c>
       <c r="D8" t="n">
-        <v>21.2087247003941</v>
+        <v>17.4393956290234</v>
       </c>
       <c r="E8" t="n">
-        <v>10.901569176131</v>
+        <v>-1.79893411995474</v>
       </c>
       <c r="F8" t="n">
-        <v>31.5510611421812</v>
+        <v>37.5154343527284</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>1118.15789473684</v>
@@ -640,16 +640,16 @@
         <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>57.9766805011587</v>
+        <v>-8.28038947203445</v>
       </c>
       <c r="E9" t="n">
-        <v>31.6400838022658</v>
+        <v>-19.5163408515315</v>
       </c>
       <c r="F9" t="n">
-        <v>95.9139171081479</v>
+        <v>4.72307014844956</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
         <v>322.263157894737</v>
@@ -669,13 +669,13 @@
         <v>14</v>
       </c>
       <c r="D10" t="n">
-        <v>56.5810737412604</v>
+        <v>30.2771796723165</v>
       </c>
       <c r="E10" t="n">
-        <v>30.3455798234838</v>
+        <v>2.19610836858658</v>
       </c>
       <c r="F10" t="n">
-        <v>98.506311160116</v>
+        <v>72.3575384112918</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
@@ -698,13 +698,13 @@
         <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>-16.8657393725726</v>
+        <v>-35.399702251583</v>
       </c>
       <c r="E11" t="n">
-        <v>-25.1307165779118</v>
+        <v>-45.6850735016055</v>
       </c>
       <c r="F11" t="n">
-        <v>-6.77511780061891</v>
+        <v>-24.4221172343063</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
@@ -727,13 +727,13 @@
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>3.43294638693178</v>
+        <v>2.583994687556</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.65012984413163</v>
+        <v>-2.83512997346274</v>
       </c>
       <c r="F12" t="n">
-        <v>7.76134619583574</v>
+        <v>15.926019401117</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -756,16 +756,16 @@
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>19.8472512305629</v>
+        <v>12.2421704294136</v>
       </c>
       <c r="E13" t="n">
-        <v>6.69157486838403</v>
+        <v>-9.43489729406951</v>
       </c>
       <c r="F13" t="n">
-        <v>34.1299304695193</v>
+        <v>32.8294924459343</v>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
         <v>2220.52631578947</v>
@@ -785,16 +785,16 @@
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>120.130500317897</v>
+        <v>-9.1240236681981</v>
       </c>
       <c r="E14" t="n">
-        <v>63.7314956449412</v>
+        <v>-24.5638658121862</v>
       </c>
       <c r="F14" t="n">
-        <v>214.822381699593</v>
+        <v>11.4586564566882</v>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
         <v>375.315789473684</v>
@@ -814,16 +814,16 @@
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>210.557828156942</v>
+        <v>155.692560143525</v>
       </c>
       <c r="E15" t="n">
-        <v>97.0460216264289</v>
+        <v>-32.4910791518741</v>
       </c>
       <c r="F15" t="n">
-        <v>398.826930346321</v>
+        <v>456.821493404389</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
         <v>193.736842105263</v>
@@ -843,13 +843,13 @@
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>145.771235644729</v>
+        <v>144.296975829521</v>
       </c>
       <c r="E16" t="n">
-        <v>83.5447401488224</v>
+        <v>80.2760983568056</v>
       </c>
       <c r="F16" t="n">
-        <v>230.641682750723</v>
+        <v>243.092071745791</v>
       </c>
       <c r="G16" t="n">
         <v>1</v>
@@ -872,16 +872,16 @@
         <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>4.07448859494469</v>
+        <v>-1.85552939885885</v>
       </c>
       <c r="E17" t="n">
-        <v>0.839500229598382</v>
+        <v>-5.30487659806178</v>
       </c>
       <c r="F17" t="n">
-        <v>7.50010627375154</v>
+        <v>2.34537255745965</v>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
         <v>9147.52631578947</v>
@@ -901,16 +901,16 @@
         <v>12</v>
       </c>
       <c r="D18" t="n">
-        <v>21.9194187208039</v>
+        <v>10.6995046902919</v>
       </c>
       <c r="E18" t="n">
-        <v>13.9518720111582</v>
+        <v>-14.42401903237</v>
       </c>
       <c r="F18" t="n">
-        <v>31.3962266751789</v>
+        <v>28.3404294696575</v>
       </c>
       <c r="G18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
         <v>2254.15789473684</v>
@@ -930,13 +930,13 @@
         <v>13</v>
       </c>
       <c r="D19" t="n">
-        <v>76.7214989760613</v>
+        <v>26.5230956547787</v>
       </c>
       <c r="E19" t="n">
-        <v>53.4462798150482</v>
+        <v>3.24128791090334</v>
       </c>
       <c r="F19" t="n">
-        <v>105.219584370388</v>
+        <v>83.5406242053416</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
@@ -959,16 +959,16 @@
         <v>14</v>
       </c>
       <c r="D20" t="n">
-        <v>66.9266910978088</v>
+        <v>34.0914256627225</v>
       </c>
       <c r="E20" t="n">
-        <v>31.2964152129587</v>
+        <v>-3.34258407504167</v>
       </c>
       <c r="F20" t="n">
-        <v>117.638330980901</v>
+        <v>102.62496920381</v>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
         <v>284.105263157895</v>
@@ -988,13 +988,13 @@
         <v>15</v>
       </c>
       <c r="D21" t="n">
-        <v>-43.4121490548788</v>
+        <v>-41.3131527556954</v>
       </c>
       <c r="E21" t="n">
-        <v>-48.6899213714106</v>
+        <v>-52.1883779473875</v>
       </c>
       <c r="F21" t="n">
-        <v>-36.7459298937381</v>
+        <v>-27.6604294665201</v>
       </c>
       <c r="G21" t="n">
         <v>1</v>

</xml_diff>